<commit_message>
update TarisSG and TechGlobal
</commit_message>
<xml_diff>
--- a/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2021/Thang5/02.XuLyBH/XLBH2105_TarisSG.xlsx
+++ b/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2021/Thang5/02.XuLyBH/XLBH2105_TarisSG.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PhongBaoHanh\VNET\5. WS\1. Bộ phận bảo hành\1. Thực hiện sửa chữa bảo hành\nam2021\Thang5\02.XuLyBH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VNET\5. WS\1. Bộ phận bảo hành\1. Thực hiện sửa chữa bảo hành\nam2021\Thang5\02.XuLyBH\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="183">
   <si>
     <t>STT</t>
   </si>
@@ -525,10 +525,67 @@
     <t>W.1.00.---01.180629</t>
   </si>
   <si>
-    <t>112.213.94.88,31001</t>
-  </si>
-  <si>
     <t>Thay khay sim cho thiết bị, nâng cấp FW</t>
+  </si>
+  <si>
+    <t>Tùng</t>
+  </si>
+  <si>
+    <t>Lock: 112.213.94.88,31001</t>
+  </si>
+  <si>
+    <t>Thiết bị mất cấu hình</t>
+  </si>
+  <si>
+    <t>Nạp lại FW, nâng cấp khay sim</t>
+  </si>
+  <si>
+    <t>LK,MCH</t>
+  </si>
+  <si>
+    <t>Nâng cấp khay sim, nâng cấp FW</t>
+  </si>
+  <si>
+    <t>Lock: 203.162.69.75,20575</t>
+  </si>
+  <si>
+    <t>Thiết bị reset liên tục</t>
+  </si>
+  <si>
+    <t>Thay thạch anh, nạp lại FW, nâng cấp FW</t>
+  </si>
+  <si>
+    <t>Lock: 203.162.69.75,30001</t>
+  </si>
+  <si>
+    <t>VI.1.00.---01.180320</t>
+  </si>
+  <si>
+    <t>Lock: 203.162.69.18,16884</t>
+  </si>
+  <si>
+    <t>Lock: 203.162.69.75,20275</t>
+  </si>
+  <si>
+    <t>Lock: 203.162.69.75,30031</t>
+  </si>
+  <si>
+    <t>Thiết bị chập ACC</t>
+  </si>
+  <si>
+    <t>Lock: 203.162.69.75,30000</t>
+  </si>
+  <si>
+    <t>Lock: 203.162.69.75,20475</t>
+  </si>
+  <si>
+    <t>Mạch oxi hóa</t>
+  </si>
+  <si>
+    <t>Không sửa chữa</t>
+  </si>
+  <si>
+    <t>Báo giá không sửa</t>
   </si>
 </sst>
 </file>
@@ -1300,8 +1357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X57"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView showZeros="0" topLeftCell="G7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21:M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2372,7 +2429,9 @@
       <c r="B21" s="69">
         <v>44342</v>
       </c>
-      <c r="C21" s="37"/>
+      <c r="C21" s="37">
+        <v>44391</v>
+      </c>
       <c r="D21" s="38" t="s">
         <v>66</v>
       </c>
@@ -2385,21 +2444,33 @@
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="57" t="s">
-        <v>98</v>
-      </c>
-      <c r="J21" s="1"/>
+        <v>172</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="K21" s="1" t="s">
         <v>159</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="M21" s="1"/>
+      <c r="M21" s="40" t="s">
+        <v>128</v>
+      </c>
       <c r="N21" s="1"/>
-      <c r="O21" s="40"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="10"/>
+      <c r="O21" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q21" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="R21" s="10" t="s">
+        <v>122</v>
+      </c>
       <c r="S21" s="4"/>
       <c r="T21" s="14"/>
       <c r="U21" s="10" t="s">
@@ -2407,7 +2478,7 @@
       </c>
       <c r="V21" s="10">
         <f>COUNTIF($Q$6:$Q$51,"PC")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W21" s="14"/>
     </row>
@@ -2418,7 +2489,9 @@
       <c r="B22" s="69">
         <v>44342</v>
       </c>
-      <c r="C22" s="37"/>
+      <c r="C22" s="37">
+        <v>44391</v>
+      </c>
       <c r="D22" s="38" t="s">
         <v>66</v>
       </c>
@@ -2431,15 +2504,27 @@
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="57"/>
-      <c r="J22" s="10"/>
+      <c r="J22" s="10" t="s">
+        <v>180</v>
+      </c>
       <c r="K22" s="10"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="10"/>
+      <c r="M22" s="10" t="s">
+        <v>181</v>
+      </c>
       <c r="N22" s="10"/>
-      <c r="O22" s="40"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="10"/>
+      <c r="O22" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="P22" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R22" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="S22" s="4"/>
       <c r="T22" s="14"/>
       <c r="U22" s="10" t="s">
@@ -2447,7 +2532,7 @@
       </c>
       <c r="V22" s="10">
         <f>COUNTIF($Q$6:$Q$51,"PC+PM")</f>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="W22" s="14"/>
     </row>
@@ -2458,7 +2543,9 @@
       <c r="B23" s="69">
         <v>44342</v>
       </c>
-      <c r="C23" s="37"/>
+      <c r="C23" s="37">
+        <v>44391</v>
+      </c>
       <c r="D23" s="38" t="s">
         <v>66</v>
       </c>
@@ -2471,15 +2558,29 @@
       </c>
       <c r="H23" s="10"/>
       <c r="I23" s="57"/>
-      <c r="J23" s="1"/>
+      <c r="J23" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
+      <c r="L23" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="M23" s="10" t="s">
+        <v>166</v>
+      </c>
       <c r="N23" s="10"/>
-      <c r="O23" s="40"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="10"/>
+      <c r="O23" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="P23" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q23" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="R23" s="10" t="s">
+        <v>167</v>
+      </c>
       <c r="S23" s="4"/>
       <c r="T23" s="14"/>
       <c r="U23" s="14"/>
@@ -2493,7 +2594,9 @@
       <c r="B24" s="69">
         <v>44342</v>
       </c>
-      <c r="C24" s="37"/>
+      <c r="C24" s="37">
+        <v>44391</v>
+      </c>
       <c r="D24" s="38" t="s">
         <v>66</v>
       </c>
@@ -2506,21 +2609,33 @@
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="57" t="s">
-        <v>103</v>
-      </c>
-      <c r="J24" s="1"/>
+        <v>176</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="K24" s="10" t="s">
         <v>160</v>
       </c>
       <c r="L24" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="M24" s="10"/>
+      <c r="M24" s="10" t="s">
+        <v>168</v>
+      </c>
       <c r="N24" s="10"/>
-      <c r="O24" s="40"/>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="10"/>
+      <c r="O24" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="P24" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q24" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="R24" s="10" t="s">
+        <v>122</v>
+      </c>
       <c r="S24" s="4"/>
       <c r="T24" s="14"/>
       <c r="U24" s="14"/>
@@ -2534,7 +2649,9 @@
       <c r="B25" s="69">
         <v>44342</v>
       </c>
-      <c r="C25" s="69"/>
+      <c r="C25" s="37">
+        <v>44391</v>
+      </c>
       <c r="D25" s="38" t="s">
         <v>66</v>
       </c>
@@ -2547,7 +2664,7 @@
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="57" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>75</v>
@@ -2558,12 +2675,22 @@
       <c r="L25" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="M25" s="10"/>
+      <c r="M25" s="40" t="s">
+        <v>128</v>
+      </c>
       <c r="N25" s="10"/>
-      <c r="O25" s="40"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="10"/>
+      <c r="O25" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="P25" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q25" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="R25" s="10" t="s">
+        <v>122</v>
+      </c>
       <c r="S25" s="4"/>
       <c r="T25" s="14"/>
       <c r="U25" s="75" t="s">
@@ -2581,7 +2708,9 @@
       <c r="B26" s="69">
         <v>44342</v>
       </c>
-      <c r="C26" s="69"/>
+      <c r="C26" s="37">
+        <v>44391</v>
+      </c>
       <c r="D26" s="38" t="s">
         <v>66</v>
       </c>
@@ -2593,16 +2722,32 @@
         <v>61</v>
       </c>
       <c r="H26" s="10"/>
-      <c r="I26" s="57"/>
-      <c r="J26" s="1"/>
+      <c r="I26" s="57" t="s">
+        <v>169</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>170</v>
+      </c>
       <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
+      <c r="L26" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="M26" s="10" t="s">
+        <v>171</v>
+      </c>
       <c r="N26" s="10"/>
-      <c r="O26" s="40"/>
-      <c r="P26" s="10"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="10"/>
+      <c r="O26" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="P26" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q26" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="R26" s="10" t="s">
+        <v>122</v>
+      </c>
       <c r="S26" s="4"/>
       <c r="T26" s="14"/>
       <c r="U26" s="4" t="s">
@@ -2621,7 +2766,9 @@
       <c r="B27" s="69">
         <v>44342</v>
       </c>
-      <c r="C27" s="69"/>
+      <c r="C27" s="37">
+        <v>44391</v>
+      </c>
       <c r="D27" s="38" t="s">
         <v>66</v>
       </c>
@@ -2633,16 +2780,34 @@
         <v>61</v>
       </c>
       <c r="H27" s="10"/>
-      <c r="I27" s="57"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
+      <c r="I27" s="57" t="s">
+        <v>174</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K27" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="L27" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="M27" s="10" t="s">
+        <v>128</v>
+      </c>
       <c r="N27" s="10"/>
-      <c r="O27" s="40"/>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="10"/>
+      <c r="O27" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="P27" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q27" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="R27" s="10" t="s">
+        <v>122</v>
+      </c>
       <c r="S27" s="4"/>
       <c r="T27" s="14"/>
       <c r="U27" s="4" t="s">
@@ -2661,7 +2826,9 @@
       <c r="B28" s="69">
         <v>44342</v>
       </c>
-      <c r="C28" s="69"/>
+      <c r="C28" s="37">
+        <v>44391</v>
+      </c>
       <c r="D28" s="38" t="s">
         <v>66</v>
       </c>
@@ -2673,16 +2840,34 @@
         <v>61</v>
       </c>
       <c r="H28" s="1"/>
-      <c r="I28" s="57"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
+      <c r="I28" s="57" t="s">
+        <v>175</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K28" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="L28" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="M28" s="10" t="s">
+        <v>128</v>
+      </c>
       <c r="N28" s="1"/>
-      <c r="O28" s="40"/>
-      <c r="P28" s="10"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="10"/>
+      <c r="O28" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="P28" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q28" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="R28" s="10" t="s">
+        <v>122</v>
+      </c>
       <c r="S28" s="4"/>
       <c r="T28" s="14"/>
       <c r="U28" s="4" t="s">
@@ -2701,7 +2886,9 @@
       <c r="B29" s="69">
         <v>44342</v>
       </c>
-      <c r="C29" s="69"/>
+      <c r="C29" s="37">
+        <v>44391</v>
+      </c>
       <c r="D29" s="38" t="s">
         <v>66</v>
       </c>
@@ -2759,7 +2946,9 @@
       <c r="B30" s="69">
         <v>44342</v>
       </c>
-      <c r="C30" s="69"/>
+      <c r="C30" s="37">
+        <v>44391</v>
+      </c>
       <c r="D30" s="38" t="s">
         <v>66</v>
       </c>
@@ -2771,16 +2960,32 @@
         <v>61</v>
       </c>
       <c r="H30" s="1"/>
-      <c r="I30" s="57"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
+      <c r="I30" s="57" t="s">
+        <v>132</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K30" s="57" t="s">
+        <v>160</v>
+      </c>
       <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
+      <c r="M30" s="1" t="s">
+        <v>168</v>
+      </c>
       <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="4"/>
-      <c r="R30" s="10"/>
+      <c r="O30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q30" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="R30" s="10" t="s">
+        <v>122</v>
+      </c>
       <c r="S30" s="4"/>
       <c r="T30" s="14"/>
       <c r="U30" s="4" t="s">
@@ -2788,7 +2993,7 @@
       </c>
       <c r="V30" s="10">
         <f>COUNTIF($R$6:$R$51,"*I/O*")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W30" s="14"/>
     </row>
@@ -2799,7 +3004,9 @@
       <c r="B31" s="69">
         <v>44342</v>
       </c>
-      <c r="C31" s="69"/>
+      <c r="C31" s="37">
+        <v>44391</v>
+      </c>
       <c r="D31" s="38" t="s">
         <v>66</v>
       </c>
@@ -2811,16 +3018,34 @@
         <v>61</v>
       </c>
       <c r="H31" s="1"/>
-      <c r="I31" s="57"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
+      <c r="I31" s="57" t="s">
+        <v>179</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L31" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>168</v>
+      </c>
       <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="10"/>
+      <c r="O31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q31" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="R31" s="10" t="s">
+        <v>122</v>
+      </c>
       <c r="S31" s="4"/>
       <c r="T31" s="14"/>
       <c r="U31" s="4" t="s">
@@ -2828,7 +3053,7 @@
       </c>
       <c r="V31" s="10">
         <f>COUNTIF($R$6:$R$51,"*LK*")</f>
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="W31" s="14"/>
     </row>
@@ -2839,7 +3064,9 @@
       <c r="B32" s="69">
         <v>44342</v>
       </c>
-      <c r="C32" s="69"/>
+      <c r="C32" s="37">
+        <v>44391</v>
+      </c>
       <c r="D32" s="38" t="s">
         <v>66</v>
       </c>
@@ -2852,15 +3079,27 @@
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="57"/>
-      <c r="J32" s="1"/>
+      <c r="J32" s="1" t="s">
+        <v>177</v>
+      </c>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="10"/>
+      <c r="M32" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="N32" s="52"/>
+      <c r="O32" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q32" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R32" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="S32" s="4"/>
       <c r="T32" s="14"/>
       <c r="U32" s="4" t="s">
@@ -2868,7 +3107,7 @@
       </c>
       <c r="V32" s="10">
         <f>COUNTIF($R$6:$R$51,"*MCH*")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W32" s="14"/>
     </row>
@@ -2879,7 +3118,9 @@
       <c r="B33" s="69">
         <v>44342</v>
       </c>
-      <c r="C33" s="69"/>
+      <c r="C33" s="37">
+        <v>44391</v>
+      </c>
       <c r="D33" s="38" t="s">
         <v>66</v>
       </c>
@@ -2891,16 +3132,34 @@
         <v>61</v>
       </c>
       <c r="H33" s="1"/>
-      <c r="I33" s="57"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
+      <c r="I33" s="57" t="s">
+        <v>178</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L33" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>168</v>
+      </c>
       <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="10"/>
+      <c r="O33" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q33" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="R33" s="10" t="s">
+        <v>122</v>
+      </c>
       <c r="S33" s="4"/>
       <c r="T33" s="14"/>
       <c r="U33" s="4" t="s">
@@ -2972,7 +3231,7 @@
       </c>
       <c r="V35" s="10">
         <f>COUNTIF($R$6:$R$51,"*NCFW*")</f>
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="W35" s="14"/>
     </row>
@@ -3036,7 +3295,7 @@
       </c>
       <c r="V37" s="10">
         <f>SUM(V26:V36)</f>
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="W37" s="14"/>
     </row>
@@ -3154,7 +3413,7 @@
       </c>
       <c r="V41" s="10">
         <f>COUNTIF($O$6:$O$51,"*KS*")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W41" s="14"/>
     </row>
@@ -5450,8 +5709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X57"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="C6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7567,7 +7826,7 @@
         <v>71</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N39" s="1"/>
       <c r="O39" s="1" t="s">

</xml_diff>